<commit_message>
Rough draft of integration of analysis into main GUI Added progress bar to analysis window
</commit_message>
<xml_diff>
--- a/Resources/Database.xlsx
+++ b/Resources/Database.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\MATLAB\DefinitiveTCM.git\Resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="1"/>
   </bookViews>
@@ -381,7 +386,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -450,7 +455,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Resolved some analysis issues to bring results to match original code
</commit_message>
<xml_diff>
--- a/Resources/Database.xlsx
+++ b/Resources/Database.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>filmgold</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>sensitivityConstant</t>
+  </si>
+  <si>
+    <t>seed</t>
   </si>
 </sst>
 </file>
@@ -451,11 +454,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6:XFD6"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,10 +488,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>115</v>
+        <v>160</v>
       </c>
       <c r="C2" s="1">
-        <v>6.0718899999999999E-5</v>
+        <v>6.4766799999999998E-5</v>
       </c>
       <c r="D2">
         <v>19300</v>
@@ -534,6 +537,17 @@
       </c>
       <c r="D5">
         <v>2649</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3.4000000000000001E-6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Crash prevention fixes Added automatic sensitivity adjustment (on request for film thickness calculations, automatically for center, focus, and data scans)
</commit_message>
<xml_diff>
--- a/Resources/Database.xlsx
+++ b/Resources/Database.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\MATLAB\DefinitiveTCM.git\Resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="1"/>
+    <workbookView xWindow="390" yWindow="4035" windowWidth="28800" windowHeight="13020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Magnification" sheetId="2" r:id="rId1"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>filmgold</t>
   </si>
@@ -69,6 +64,21 @@
   </si>
   <si>
     <t>seed</t>
+  </si>
+  <si>
+    <t>BK7</t>
+  </si>
+  <si>
+    <t>Borofloat</t>
+  </si>
+  <si>
+    <t>CaF2</t>
+  </si>
+  <si>
+    <t>ZnSe</t>
+  </si>
+  <si>
+    <t>ZnS</t>
   </si>
 </sst>
 </file>
@@ -389,7 +399,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -454,11 +464,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,10 +498,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>160</v>
+        <v>140.26300000000001</v>
       </c>
       <c r="C2" s="1">
-        <v>6.4766799999999998E-5</v>
+        <v>1.4500000000000001E-2</v>
       </c>
       <c r="D2">
         <v>19300</v>
@@ -499,54 +509,124 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B3">
-        <v>1.089</v>
+        <v>1.2</v>
       </c>
       <c r="C3" s="1">
-        <v>6.5000000000000002E-7</v>
+        <v>6.5700000000000002E-7</v>
       </c>
       <c r="D3">
-        <v>2530</v>
+        <v>2200</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B4">
-        <v>318</v>
+        <v>1.1140000000000001</v>
       </c>
       <c r="C4" s="1">
-        <v>1.27E-4</v>
+        <v>5.1667600000000004E-7</v>
       </c>
       <c r="D4">
-        <v>19300</v>
+        <v>2510</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B5">
-        <v>6.5</v>
+        <v>9.7100000000000009</v>
       </c>
       <c r="C5" s="1">
-        <v>3.3113999999999999E-7</v>
+        <v>3.5754999999999999E-6</v>
       </c>
       <c r="D5">
-        <v>2649</v>
+        <v>3180</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1.0074999999999999E-5</v>
+      </c>
+      <c r="D6">
+        <v>5270</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <v>27.2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1.2913300000000001E-5</v>
+      </c>
+      <c r="D7">
+        <v>4090</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>1.089</v>
+      </c>
+      <c r="C8" s="1">
+        <v>6.5000000000000002E-7</v>
+      </c>
+      <c r="D8">
+        <v>2530</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>318</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1.27E-4</v>
+      </c>
+      <c r="D9">
+        <v>19300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>6.5</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3.3113999999999999E-7</v>
+      </c>
+      <c r="D10">
+        <v>2649</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B6">
+      <c r="B11">
         <v>9.1999999999999993</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C11" s="1">
         <v>3.4000000000000001E-6</v>
       </c>
     </row>

</xml_diff>